<commit_message>
actualización formato para cargue
</commit_message>
<xml_diff>
--- a/balance-pix.xlsx
+++ b/balance-pix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Personal\Documentos personales\SCRIPT\Balances-Pix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABDE6E4-89EF-4C67-BCCF-FBDB263ACC5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5A6727-0C55-4745-A216-0C6131AFEC85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{12373DC2-E3C6-41F0-A981-02CBE3560ADC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>entity-id</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>clientSecret</t>
-  </si>
-  <si>
-    <t>apiKey</t>
   </si>
 </sst>
 </file>
@@ -98,10 +95,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -421,15 +414,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22C1007B-24F9-43FF-9CE1-D1FD768442E8}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -447,9 +440,6 @@
       </c>
       <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>